<commit_message>
Added all the gates grants to the application worksheet.
</commit_message>
<xml_diff>
--- a/templates/1-ApplicationInformationWorksheet.xlsx
+++ b/templates/1-ApplicationInformationWorksheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="492" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Application Information " sheetId="1" state="visible" r:id="rId2"/>
@@ -96,7 +96,14 @@
     <t>Has your institution ever received a grant from the Bill &amp; Melinda Gates Foundation?  If so, to the best of your knowledge, please list the previous grants.</t>
   </si>
   <si>
-    <t>English Department WexMooc grant</t>
+    <t>* Writing II: Rhetorical composition - MOOCs for general and developmental education 
+* A new system for dual bacterial/insecticidal crop protection 
+* Quadruplex-based technology for isothermal DNA amplification and non-enzymatic detection 
+* Bacillus-fermented natto as edible vaccines for the developing world 
+* A novel approach of creating an attenuated pneumonia vaccine 
+* New technology for production of pneumonia vaccines 
+* Gates Foundation: Ohio follow-through on Achieve policy study recommendations
+* Improving cassava for nutrition, health, and sustainable development. </t>
   </si>
   <si>
     <t>Adaptive Technology Provider Information</t>
@@ -247,7 +254,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -292,6 +299,13 @@
       <color rgb="FF000000"/>
       <sz val="11"/>
       <u val="single"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="7"/>
     </font>
   </fonts>
   <fills count="8">
@@ -379,7 +393,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -425,6 +439,10 @@
       <protection hidden="false" locked="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="false"/>
     </xf>
@@ -531,8 +549,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C31" activeCellId="0" pane="topLeft" sqref="C31"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C17" activeCellId="0" pane="topLeft" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.6"/>
@@ -662,22 +680,22 @@
       <c r="B13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30.75" outlineLevel="0" r="14">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="15">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -685,10 +703,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="16">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -696,10 +714,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -707,10 +725,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="18">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -718,10 +736,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -729,10 +747,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="15" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -740,10 +758,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="75" outlineLevel="0" r="21">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -751,17 +769,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="26.25" outlineLevel="0" r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -769,10 +787,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="9" t="s">
@@ -780,10 +798,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="9" t="s">
@@ -791,10 +809,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -802,10 +820,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -813,10 +831,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="9" t="s">
@@ -824,19 +842,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="29">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="18" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="30">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="10" t="n">
@@ -844,100 +862,100 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="31">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="32">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="33">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="34">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="35">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="36">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="37">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C37" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="38">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="39">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C39" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="40">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="41">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="18" t="s">
         <v>65</v>
       </c>
       <c r="C41" s="11"/>

</xml_diff>